<commit_message>
Updated feeder for actual format from a customer
</commit_message>
<xml_diff>
--- a/src/test/resources/data_sample.xlsx
+++ b/src/test/resources/data_sample.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="51">
   <si>
     <t xml:space="preserve">Дата/Время</t>
   </si>
@@ -88,7 +88,10 @@
     <t xml:space="preserve">СДЭК (посылка - до пункта выдачи). ул. Павших Стрелков, д. 1</t>
   </si>
   <si>
-    <t xml:space="preserve">ндс10</t>
+    <t xml:space="preserve">услуга</t>
+  </si>
+  <si>
+    <t xml:space="preserve">БЕЗ НДС</t>
   </si>
   <si>
     <t xml:space="preserve">139_6926833</t>
@@ -97,7 +100,7 @@
     <t xml:space="preserve">Больше, чем бизнес. Как преодолеть ограничения и построить великую компанию. Коллинз Дж.</t>
   </si>
   <si>
-    <t xml:space="preserve">ндс20</t>
+    <t xml:space="preserve">товар</t>
   </si>
   <si>
     <t xml:space="preserve">139_7009505</t>
@@ -106,9 +109,6 @@
     <t xml:space="preserve">ДУМАЙ И БОГАТЕЙ! Самое полное издание, исправленное и дополненное</t>
   </si>
   <si>
-    <t xml:space="preserve">ндс0</t>
-  </si>
-  <si>
     <t xml:space="preserve">ОСПИЧЕВ ДМИТРИЙ ВАСИЛЬЕВИЧ</t>
   </si>
   <si>
@@ -119,9 +119,6 @@
   </si>
   <si>
     <t xml:space="preserve">Почта России (курьер онлайн - до двери). 443000, Самара, Блюхера , 19, 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ндсНет</t>
   </si>
   <si>
     <t xml:space="preserve">139_4387596</t>
@@ -186,7 +183,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd\.mm\.yyyy\ h:mm"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -230,6 +227,12 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -323,11 +326,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -410,11 +413,11 @@
   </sheetPr>
   <dimension ref="A1:O16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G22" activeCellId="0" sqref="G22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q10" activeCellId="0" sqref="Q10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.14"/>
@@ -539,11 +542,11 @@
         <v>44362.66875</v>
       </c>
       <c r="M3" s="6"/>
-      <c r="N3" s="6" t="n">
-        <v>4</v>
+      <c r="N3" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="O3" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -554,7 +557,7 @@
         <v>48689</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>16</v>
@@ -566,7 +569,7 @@
         <v>18</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H4" s="8" t="n">
         <v>1</v>
@@ -578,11 +581,11 @@
         <v>44362.66875</v>
       </c>
       <c r="M4" s="6"/>
-      <c r="N4" s="6" t="n">
-        <v>1</v>
+      <c r="N4" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="O4" s="0" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -593,7 +596,7 @@
         <v>48689</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>16</v>
@@ -605,7 +608,7 @@
         <v>18</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H5" s="8" t="n">
         <v>1</v>
@@ -617,11 +620,11 @@
         <v>44362.66875</v>
       </c>
       <c r="M5" s="6"/>
-      <c r="N5" s="6" t="n">
-        <v>1</v>
+      <c r="N5" s="9" t="s">
+        <v>26</v>
       </c>
       <c r="O5" s="0" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -659,6 +662,9 @@
         <v>31</v>
       </c>
       <c r="N6" s="6"/>
+      <c r="O6" s="0" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="n">
@@ -692,11 +698,11 @@
         <v>44384.8604166667</v>
       </c>
       <c r="M7" s="6"/>
-      <c r="N7" s="6" t="n">
-        <v>4</v>
+      <c r="N7" s="9" t="s">
+        <v>22</v>
       </c>
       <c r="O7" s="0" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -707,7 +713,7 @@
         <v>49079</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>29</v>
@@ -719,7 +725,7 @@
         <v>18</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H8" s="8" t="n">
         <v>1</v>
@@ -731,11 +737,11 @@
         <v>44384.8604166667</v>
       </c>
       <c r="M8" s="6"/>
-      <c r="N8" s="6" t="n">
-        <v>1</v>
+      <c r="N8" s="9" t="s">
+        <v>26</v>
       </c>
       <c r="O8" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -746,7 +752,7 @@
         <v>49079</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>29</v>
@@ -758,7 +764,7 @@
         <v>18</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H9" s="8" t="n">
         <v>1</v>
@@ -770,11 +776,11 @@
         <v>44384.8604166667</v>
       </c>
       <c r="M9" s="6"/>
-      <c r="N9" s="6" t="n">
-        <v>1</v>
+      <c r="N9" s="9" t="s">
+        <v>26</v>
       </c>
       <c r="O9" s="0" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -788,10 +794,10 @@
         <v>15</v>
       </c>
       <c r="D10" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>39</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>18</v>
@@ -808,10 +814,13 @@
       <c r="L10" s="3" t="n">
         <v>44386.0076388889</v>
       </c>
-      <c r="M10" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="N10" s="9"/>
+      <c r="M10" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="N10" s="10"/>
+      <c r="O10" s="0" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="n">
@@ -824,16 +833,16 @@
         <v>20</v>
       </c>
       <c r="D11" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="8" t="s">
-        <v>39</v>
-      </c>
       <c r="F11" s="4" t="s">
         <v>18</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H11" s="8" t="n">
         <v>1</v>
@@ -845,11 +854,11 @@
         <v>44386.0076388889</v>
       </c>
       <c r="M11" s="6"/>
-      <c r="N11" s="6" t="n">
-        <v>4</v>
-      </c>
-      <c r="O11" s="10" t="s">
-        <v>28</v>
+      <c r="N11" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="O11" s="0" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -860,19 +869,19 @@
         <v>49113</v>
       </c>
       <c r="C12" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G12" s="8" t="s">
         <v>42</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>43</v>
       </c>
       <c r="H12" s="8" t="n">
         <v>1</v>
@@ -884,11 +893,11 @@
         <v>44386.0076388889</v>
       </c>
       <c r="M12" s="6"/>
-      <c r="N12" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="O12" s="10" t="s">
-        <v>33</v>
+      <c r="N12" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="O12" s="0" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -899,19 +908,19 @@
         <v>49113</v>
       </c>
       <c r="C13" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G13" s="8" t="s">
         <v>44</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>45</v>
       </c>
       <c r="H13" s="8" t="n">
         <v>1</v>
@@ -923,11 +932,11 @@
         <v>44386.0076388889</v>
       </c>
       <c r="M13" s="6"/>
-      <c r="N13" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="O13" s="10" t="s">
-        <v>22</v>
+      <c r="N13" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="O13" s="0" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -941,10 +950,10 @@
         <v>15</v>
       </c>
       <c r="D14" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>47</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>18</v>
@@ -961,10 +970,13 @@
       <c r="L14" s="3" t="n">
         <v>44386.1798611111</v>
       </c>
-      <c r="M14" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="N14" s="9"/>
+      <c r="M14" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="N14" s="10"/>
+      <c r="O14" s="0" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="7" t="n">
@@ -977,16 +989,16 @@
         <v>20</v>
       </c>
       <c r="D15" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E15" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="E15" s="8" t="s">
-        <v>47</v>
-      </c>
       <c r="F15" s="4" t="s">
         <v>18</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H15" s="8" t="n">
         <v>1</v>
@@ -998,11 +1010,11 @@
         <v>44386.1798611111</v>
       </c>
       <c r="M15" s="6"/>
-      <c r="N15" s="6" t="n">
-        <v>4</v>
+      <c r="N15" s="9" t="s">
+        <v>22</v>
       </c>
       <c r="O15" s="0" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1013,19 +1025,19 @@
         <v>49115</v>
       </c>
       <c r="C16" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" s="8" t="s">
         <v>50</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>51</v>
       </c>
       <c r="H16" s="8" t="n">
         <v>1</v>
@@ -1037,30 +1049,30 @@
         <v>44386.1798611111</v>
       </c>
       <c r="M16" s="6"/>
-      <c r="N16" s="6" t="n">
-        <v>1</v>
+      <c r="N16" s="9" t="s">
+        <v>26</v>
       </c>
       <c r="O16" s="0" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" display="sergey@ecomkassa"/>
-    <hyperlink ref="F3" r:id="rId2" display="sergey@ecomkassa"/>
-    <hyperlink ref="F4" r:id="rId3" display="sergey@ecomkassa"/>
-    <hyperlink ref="F5" r:id="rId4" display="sergey@ecomkassa"/>
-    <hyperlink ref="F6" r:id="rId5" display="sergey@ecomkassa"/>
-    <hyperlink ref="F7" r:id="rId6" display="sergey@ecomkassa"/>
-    <hyperlink ref="F8" r:id="rId7" display="sergey@ecomkassa"/>
-    <hyperlink ref="F9" r:id="rId8" display="sergey@ecomkassa"/>
-    <hyperlink ref="F10" r:id="rId9" display="sergey@ecomkassa"/>
-    <hyperlink ref="F11" r:id="rId10" display="sergey@ecomkassa"/>
-    <hyperlink ref="F12" r:id="rId11" display="sergey@ecomkassa"/>
-    <hyperlink ref="F13" r:id="rId12" display="sergey@ecomkassa"/>
-    <hyperlink ref="F14" r:id="rId13" display="sergey@ecomkassa"/>
-    <hyperlink ref="F15" r:id="rId14" display="sergey@ecomkassa"/>
-    <hyperlink ref="F16" r:id="rId15" display="sergey@ecomkassa"/>
+    <hyperlink ref="F2" r:id="rId1" display="sergey@ecomkassa.ru"/>
+    <hyperlink ref="F3" r:id="rId2" display="sergey@ecomkassa.ru"/>
+    <hyperlink ref="F4" r:id="rId3" display="sergey@ecomkassa.ru"/>
+    <hyperlink ref="F5" r:id="rId4" display="sergey@ecomkassa.ru"/>
+    <hyperlink ref="F6" r:id="rId5" display="sergey@ecomkassa.ru"/>
+    <hyperlink ref="F7" r:id="rId6" display="sergey@ecomkassa.ru"/>
+    <hyperlink ref="F8" r:id="rId7" display="sergey@ecomkassa.ru"/>
+    <hyperlink ref="F9" r:id="rId8" display="sergey@ecomkassa.ru"/>
+    <hyperlink ref="F10" r:id="rId9" display="sergey@ecomkassa.ru"/>
+    <hyperlink ref="F11" r:id="rId10" display="sergey@ecomkassa.ru"/>
+    <hyperlink ref="F12" r:id="rId11" display="sergey@ecomkassa.ru"/>
+    <hyperlink ref="F13" r:id="rId12" display="sergey@ecomkassa.ru"/>
+    <hyperlink ref="F14" r:id="rId13" display="sergey@ecomkassa.ru"/>
+    <hyperlink ref="F15" r:id="rId14" display="sergey@ecomkassa.ru"/>
+    <hyperlink ref="F16" r:id="rId15" display="sergey@ecomkassa.ru"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>